<commit_message>
feat: migrate to pymodbus 3.11.4 and update bioyond configs
PyModbus 3.x Migration:
- Copied modbus.py and client.py from dev branch for compatibility
- Rewrote FLOAT32 decoding using struct module in coin_cell_assembly.py
- Fixed STRING decoding for QR codes (battery and electrolyte barcodes)
- Tested successfully on hardware with correct data decoding

Bioyond Studio Updates:
- Updated bioyond_studio config.py
- Modified bioyond_cell_workstation.py
- Enhanced warehouse.py and decks.py
- Added README_WAREHOUSE.md documentation

Parameter Enhancements:
- Enhanced coin_cell_workstation.yaml parameter descriptions
- Added matrix position ranges and indexing rules

Breaking changes:
- Requires pymodbus >= 3.9.0
- Removed deprecated BinaryPayloadDecoder/BinaryPayloadBuilder
- Updated to use client.convert_from/to_registers() methods
</commit_message>
<xml_diff>
--- a/unilabos/devices/workstation/bioyond_studio/bioyond_cell/material_template.xlsx
+++ b/unilabos/devices/workstation/bioyond_studio/bioyond_cell/material_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniLab\Uni-Lab-OS\unilabos\devices\workstation\bioyond_studio\bioyond_cell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4F9C2-1BBA-4508-9704-C9A82C5C5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4F680A-4780-480A-8E79-EFEC4B040FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="38">
   <si>
     <t>四号手套箱堆栈</t>
   </si>
@@ -144,7 +144,7 @@
     <t>15</t>
   </si>
   <si>
-    <t>LiFSI</t>
+    <t>TEST1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +541,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
@@ -588,8 +588,8 @@
       <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="G2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -1159,7 +1159,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="A30:I40 G26:I29 A26:E29 A17:I25 A15:E16 A3:I14 G2:I2 A2:E2 A1:I1" numberStoredAsText="1"/>
+    <ignoredError sqref="A30:I40 G26:I29 A26:E29 A17:I25 A15:E16 A3:I14 H2:I2 A2:E2 A1:I1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>